<commit_message>
mys fatura tarih güncellemesi
</commit_message>
<xml_diff>
--- a/imza.xlsx
+++ b/imza.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\vsCode\mySplit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9174C4F-8A7E-4AB6-8260-9B3F81B01A11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33D77918-2CFE-4246-8BDE-C1CA1FFF68D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -492,7 +492,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
adm ile ilgili düzeltmeler 1
</commit_message>
<xml_diff>
--- a/imza.xlsx
+++ b/imza.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\vsCode\mySplit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33D77918-2CFE-4246-8BDE-C1CA1FFF68D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B60603E-1A04-4C21-8A08-3D2B90B8F2D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -474,7 +474,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>